<commit_message>
Autonomouses Added At Waterloo - NO TESTING
NOT TESTED - updated autonomous and turret tilt, as well as Waterloo
shooting values
</commit_message>
<xml_diff>
--- a/2016CompetitionBot/Documentation/Camera Calibration Worksheet.xlsx
+++ b/2016CompetitionBot/Documentation/Camera Calibration Worksheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t xml:space="preserve">FRC 4917 Vision Camera Calibration</t>
   </si>
@@ -63,6 +63,18 @@
     <t xml:space="preserve">(enc ticks)</t>
   </si>
   <si>
+    <t xml:space="preserve">Left Side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unsure</t>
+  </si>
+  <si>
     <t xml:space="preserve">Valid Points</t>
   </si>
   <si>
@@ -81,9 +93,6 @@
     <t xml:space="preserve">Coef</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotate</t>
-  </si>
-  <si>
     <t xml:space="preserve">- Coefficient Formulas:  http://www.exceltoolset.com/getting-coefficients-of-chart-trendline/</t>
   </si>
   <si>
@@ -106,6 +115,27 @@
   </si>
   <si>
     <t xml:space="preserve">Inverted Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tilt Original</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tilt New</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dist now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dist old</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dist older</t>
   </si>
 </sst>
 </file>
@@ -116,7 +146,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -195,6 +225,11 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -262,7 +297,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -279,15 +314,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -311,20 +338,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -347,16 +366,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -392,7 +403,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF878787"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -423,10 +434,10 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FFA6A6A6"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -439,7 +450,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -549,19 +560,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.52</c:v>
+                  <c:v>1.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5</c:v>
+                  <c:v>2.53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.88</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.43</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>1.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -573,19 +584,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>66</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>75</c:v>
+                  <c:v>99.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>79.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -654,19 +665,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.45</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.52</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.76</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -678,13 +689,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>69</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -697,11 +708,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="11106509"/>
-        <c:axId val="35656892"/>
+        <c:axId val="50513946"/>
+        <c:axId val="73194456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="11106509"/>
+        <c:axId val="50513946"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,12 +786,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35656892"/>
+        <c:crossAx val="73194456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="35656892"/>
+        <c:axId val="73194456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -864,7 +875,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11106509"/>
+        <c:crossAx val="50513946"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -909,7 +920,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1020,19 +1031,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>109</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>166</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1044,19 +1055,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.52</c:v>
+                  <c:v>1.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5</c:v>
+                  <c:v>2.53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.88</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>1.43</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>1.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1126,19 +1137,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>107</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>170</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1150,13 +1161,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.45</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.52</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.76</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -1169,11 +1180,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="93556516"/>
-        <c:axId val="77397947"/>
+        <c:axId val="89543635"/>
+        <c:axId val="2616396"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93556516"/>
+        <c:axId val="89543635"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1247,12 +1258,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77397947"/>
+        <c:crossAx val="2616396"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77397947"/>
+        <c:axId val="2616396"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1336,7 +1347,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93556516"/>
+        <c:crossAx val="89543635"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1381,7 +1392,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1492,19 +1503,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.52</c:v>
+                  <c:v>1.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5</c:v>
+                  <c:v>2.53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.88</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.43</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>1.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1598,19 +1609,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.45</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.52</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.76</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1622,13 +1633,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1235</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1665</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1702</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -1641,11 +1652,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="79275442"/>
-        <c:axId val="27913901"/>
+        <c:axId val="93829469"/>
+        <c:axId val="98186946"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79275442"/>
+        <c:axId val="93829469"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1719,12 +1730,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27913901"/>
+        <c:crossAx val="98186946"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="27913901"/>
+        <c:axId val="98186946"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1808,7 +1819,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79275442"/>
+        <c:crossAx val="93829469"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1853,6 +1864,294 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tilt Original</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$A$2:$A$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1234.9999995925</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1667.2793263213</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1694.94767308</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tilt New</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$A$2:$A$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1404.00579</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2171.7437484</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2436.68744</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="78524585"/>
+        <c:axId val="54563565"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="78524585"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="54563565"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="54563565"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="78524585"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -1860,13 +2159,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>14400</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>55080</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>533160</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>131040</xdr:rowOff>
+      <xdr:colOff>532800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1875,7 +2174,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="14400" y="3943080"/>
-        <a:ext cx="4762800" cy="2742840"/>
+        <a:ext cx="4808160" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1890,13 +2189,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>19080</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>55080</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>504360</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>131040</xdr:rowOff>
+      <xdr:colOff>504000</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1904,8 +2203,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4872960" y="3943080"/>
-        <a:ext cx="4798080" cy="2742840"/>
+        <a:off x="4926240" y="3943080"/>
+        <a:ext cx="4851000" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1919,14 +2218,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>518760</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:colOff>518400</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>77760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1935,11 +2234,46 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="6791040"/>
-        <a:ext cx="4762800" cy="2743200"/>
+        <a:ext cx="4808160" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>36360</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>36000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>240840</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>98280</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="1887840" y="36000"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1953,26 +2287,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.9081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.75"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.10204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0663265306122"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="10.9081632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.2857142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.28571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1991,15 +2325,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -2030,365 +2365,406 @@
       <c r="K6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="6"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
+      <c r="A8" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="8" t="n">
-        <v>1.52</v>
-      </c>
-      <c r="C8" s="8" t="n">
-        <v>66</v>
-      </c>
-      <c r="D8" s="8" t="n">
-        <v>37</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="G8" s="7" t="n">
+      <c r="B8" s="6" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>97</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="G8" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="8" t="n">
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="0" t="n">
+        <v>5140</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>99.5</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>92</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="G9" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>106</v>
+      </c>
+      <c r="D10" s="6" t="n">
+        <v>144</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="G10" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="0" t="n">
+        <v>5432</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="C11" s="6" t="n">
+        <v>85</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="G11" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6" t="n">
         <v>1.45</v>
       </c>
-      <c r="I8" s="8" t="n">
-        <v>69</v>
-      </c>
-      <c r="J8" s="8" t="n">
-        <v>24</v>
-      </c>
-      <c r="K8" s="8" t="n">
-        <v>1235</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" s="8" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="C9" s="8" t="n">
-        <v>75</v>
-      </c>
-      <c r="D9" s="8" t="n">
-        <v>109</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="G9" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>2.52</v>
-      </c>
-      <c r="I9" s="8" t="n">
-        <v>80</v>
-      </c>
-      <c r="J9" s="8" t="n">
-        <v>107</v>
-      </c>
-      <c r="K9" s="8" t="n">
-        <v>1665</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B10" s="8" t="n">
-        <v>3.88</v>
-      </c>
-      <c r="C10" s="8" t="n">
-        <v>80</v>
-      </c>
-      <c r="D10" s="8" t="n">
-        <v>166</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="G10" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H10" s="8" t="n">
-        <v>3.76</v>
-      </c>
-      <c r="I10" s="8" t="n">
-        <v>85</v>
-      </c>
-      <c r="J10" s="8" t="n">
-        <v>170</v>
-      </c>
-      <c r="K10" s="8" t="n">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="G11" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
+      <c r="C12" s="6" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <v>29</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="G12" s="7" t="n">
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9" t="n">
+        <f aca="false">COUNT(C8:C12)</f>
         <v>5</v>
       </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11" t="n">
-        <f aca="false">COUNT(C8:C12)</f>
-        <v>3</v>
-      </c>
-      <c r="D13" s="11" t="n">
+      <c r="D13" s="9" t="n">
         <f aca="false">COUNT(D8:D12)</f>
-        <v>3</v>
-      </c>
-      <c r="E13" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" s="9" t="n">
         <f aca="false">COUNT(E8:E12)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9" t="n">
+        <f aca="false">COUNT(I8:I12)</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="9" t="n">
+        <f aca="false">COUNT(J8:J12)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="9" t="n">
+        <f aca="false">COUNT(K8:K12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="G15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="M15" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="11" t="n">
-        <f aca="false">COUNT(I8:I12)</f>
-        <v>3</v>
-      </c>
-      <c r="J13" s="11" t="n">
-        <f aca="false">COUNT(J8:J12)</f>
-        <v>3</v>
-      </c>
-      <c r="K13" s="11" t="n">
-        <f aca="false">COUNT(K8:K12)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="M15" s="17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="18" t="s">
+      <c r="F16" s="15"/>
+      <c r="G16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="18" t="s">
+      <c r="K16" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N16" s="20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="22" t="n">
+      <c r="N16" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="D17" s="22" t="n">
+      <c r="D17" s="17" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(B8,0,0,D13),OFFSET(D8,0,0,D13)^{1,2}),1)</f>
-        <v>8.2166009338592E-005</v>
-      </c>
-      <c r="E17" s="22" t="e">
+        <v>8.24107322300553E-005</v>
+      </c>
+      <c r="E17" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(E8,0,0,E13),OFFSET(B8,0,0,E13)^{1,2}),1)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="22" t="n">
+      <c r="F17" s="17"/>
+      <c r="G17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="J17" s="22" t="n">
+      <c r="J17" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(H8,0,0,J13),OFFSET(J8,0,0,J13)^{1,2}),1)</f>
-        <v>4.65135165580784E-005</v>
-      </c>
-      <c r="K17" s="22" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K17" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(K8,0,0,K13),OFFSET(H8,0,0,K13)^{1,2}),1)</f>
-        <v>-161.052142511292</v>
-      </c>
-      <c r="N17" s="20" t="s">
-        <v>22</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N17" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="22" t="n">
+      <c r="A18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="17" t="n">
         <f aca="true">SLOPE(OFFSET(C8,0,0,C13),OFFSET(B8,0,0,C13))</f>
-        <v>5.78108697714123</v>
-      </c>
-      <c r="D18" s="22" t="n">
+        <v>8.96356510378865</v>
+      </c>
+      <c r="D18" s="17" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(B8,0,0,D13),OFFSET(D8,0,0,D13)^{1,2}),1,2)</f>
-        <v>0.00161487374767669</v>
-      </c>
-      <c r="E18" s="22" t="e">
+        <v>0.00540917043605021</v>
+      </c>
+      <c r="E18" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(E8,0,0,E13),OFFSET(B8,0,0,E13)^{1,2}),1,2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="22" t="n">
+      <c r="G18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="17" t="e">
         <f aca="true">SLOPE(OFFSET(I8,0,0,I13),OFFSET(H8,0,0,I13))</f>
-        <v>6.85032299902726</v>
-      </c>
-      <c r="J18" s="22" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J18" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(H8,0,0,J13),OFFSET(J8,0,0,J13)^{1,2}),1,2)</f>
-        <v>0.00679829559595196</v>
-      </c>
-      <c r="K18" s="22" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K18" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(K8,0,0,K13),OFFSET(H8,0,0,K13)^{1,2}),1,2)</f>
-        <v>1041.24616464834</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="22" t="n">
+      <c r="A19" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="17" t="n">
         <f aca="true">INTERCEPT(OFFSET(C8,0,0,C13),OFFSET(B8,0,0,C13))</f>
-        <v>58.4431376268614</v>
-      </c>
-      <c r="D19" s="22" t="n">
+        <v>73.9490637247786</v>
+      </c>
+      <c r="D19" s="17" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(B8,0,0,D13),OFFSET(D8,0,0,D13)^{1,2}),1,3)</f>
-        <v>1.34776440455143</v>
-      </c>
-      <c r="E19" s="22" t="e">
+        <v>1.3180798365994</v>
+      </c>
+      <c r="E19" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(E8,0,0,E13),OFFSET(B8,0,0,E13)^{1,2}),1,3)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="22" t="n">
+      <c r="G19" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="17" t="e">
         <f aca="true">INTERCEPT(OFFSET(I8,0,0,I13),OFFSET(H8,0,0,I13))</f>
-        <v>60.3490010725064</v>
-      </c>
-      <c r="J19" s="22" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J19" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(H8,0,0,J13),OFFSET(J8,0,0,J13)^{1,2}),1,3)</f>
-        <v>1.2600491201597</v>
-      </c>
-      <c r="K19" s="22" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K19" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(K8,0,0,K13),OFFSET(H8,0,0,K13)^{1,2}),1,3)</f>
-        <v>63.8051908899049</v>
-      </c>
-    </row>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2414,19 +2790,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G3" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2442,109 +2818,109 @@
       <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24" t="s">
-        <v>27</v>
+      <c r="G4" s="3"/>
+      <c r="H4" s="18" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="n">
+      <c r="A5" s="6" t="n">
         <v>1.5</v>
       </c>
-      <c r="B5" s="25" t="n">
+      <c r="B5" s="19" t="n">
         <f aca="false">IF($A5&lt;&gt;"",($A5*$A5*Calibration!C$17)+($A5*Calibration!C$18)+Calibration!C$19,"")</f>
-        <v>67.1147680925733</v>
-      </c>
-      <c r="C5" s="25" t="n">
+        <v>87.3944113804616</v>
+      </c>
+      <c r="C5" s="19" t="n">
         <f aca="false">IF($A5&lt;&gt;"",($A5*$A5*$H$5)+($A5*$H$6)+$H$7,"")</f>
-        <v>35.2580271607538</v>
-      </c>
-      <c r="D5" s="25" t="e">
+        <v>24.4722094362834</v>
+      </c>
+      <c r="D5" s="19" t="e">
         <f aca="false">IF($A5&lt;&gt;"",($A5*$A5*Calibration!E$17)+($A5*Calibration!E$18)+Calibration!E$19,"")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G5" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="25" t="n">
+      <c r="G5" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="19" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(Calibration!D8,0,0,Calibration!D13),OFFSET(Calibration!B8,0,0,Calibration!D13)^{1,2}),1)</f>
-        <v>-13.6292542072098</v>
+        <v>-10.5503267320325</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="n">
+      <c r="A6" s="6" t="n">
         <v>2.5</v>
       </c>
-      <c r="B6" s="25" t="n">
+      <c r="B6" s="19" t="n">
         <f aca="false">IF($A6&lt;&gt;"",($A6*$A6*Calibration!C$17)+($A6*Calibration!C$18)+Calibration!C$19,"")</f>
-        <v>72.8958550697145</v>
-      </c>
-      <c r="C6" s="25" t="n">
+        <v>96.3579764842503</v>
+      </c>
+      <c r="C6" s="19" t="n">
         <f aca="false">IF($A6&lt;&gt;"",($A6*$A6*$H$5)+($A6*$H$6)+$H$7,"")</f>
-        <v>109</v>
-      </c>
-      <c r="D6" s="25" t="e">
+        <v>90.1690115647921</v>
+      </c>
+      <c r="D6" s="19" t="e">
         <f aca="false">IF($A6&lt;&gt;"",($A6*$A6*Calibration!E$17)+($A6*Calibration!E$18)+Calibration!E$19,"")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G6" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="25" t="n">
+      <c r="G6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="19" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(Calibration!D8,0,0,Calibration!D13),OFFSET(Calibration!B8,0,0,Calibration!D13)^{1,2}),1,2)</f>
-        <v>128.258989668085</v>
+        <v>107.898109056639</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="n">
+      <c r="A7" s="6" t="n">
         <v>3.5</v>
       </c>
-      <c r="B7" s="25" t="n">
+      <c r="B7" s="19" t="n">
         <f aca="false">IF($A7&lt;&gt;"",($A7*$A7*Calibration!C$17)+($A7*Calibration!C$18)+Calibration!C$19,"")</f>
-        <v>78.6769420468557</v>
-      </c>
-      <c r="C7" s="25" t="n">
+        <v>105.321541588039</v>
+      </c>
+      <c r="C7" s="19" t="n">
         <f aca="false">IF($A7&lt;&gt;"",($A7*$A7*$H$5)+($A7*$H$6)+$H$7,"")</f>
-        <v>155.483464424827</v>
-      </c>
-      <c r="D7" s="25" t="e">
+        <v>134.765160229236</v>
+      </c>
+      <c r="D7" s="19" t="e">
         <f aca="false">IF($A7&lt;&gt;"",($A7*$A7*Calibration!E$17)+($A7*Calibration!E$18)+Calibration!E$19,"")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G7" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="25" t="n">
+      <c r="G7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="19" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(Calibration!D8,0,0,Calibration!D13),OFFSET(Calibration!B8,0,0,Calibration!D13)^{1,2}),1,3)</f>
-        <v>-126.464635375152</v>
+        <v>-113.636719001601</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8"/>
-      <c r="B8" s="25" t="str">
+      <c r="A8" s="6"/>
+      <c r="B8" s="19" t="str">
         <f aca="false">IF($A8&lt;&gt;"",($A8*$A8*Calibration!C$17)+($A8*Calibration!C$18)+Calibration!C$19,"")</f>
         <v/>
       </c>
-      <c r="C8" s="25" t="str">
+      <c r="C8" s="19" t="str">
         <f aca="false">IF($A8&lt;&gt;"",($A8*$A8*$H$5)+($A8*$H$6)+$H$7,"")</f>
         <v/>
       </c>
-      <c r="D8" s="25" t="str">
+      <c r="D8" s="19" t="str">
         <f aca="false">IF($A8&lt;&gt;"",($A8*$A8*Calibration!E$17)+($A8*Calibration!E$18)+Calibration!E$19,"")</f>
         <v/>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8"/>
-      <c r="B9" s="25" t="str">
+      <c r="A9" s="6"/>
+      <c r="B9" s="19" t="str">
         <f aca="false">IF($A9&lt;&gt;"",($A9*$A9*Calibration!C$17)+($A9*Calibration!C$18)+Calibration!C$19,"")</f>
         <v/>
       </c>
-      <c r="C9" s="25" t="str">
+      <c r="C9" s="19" t="str">
         <f aca="false">IF($A9&lt;&gt;"",($A9*$A9*$H$5)+($A9*$H$6)+$H$7,"")</f>
         <v/>
       </c>
-      <c r="D9" s="25" t="str">
+      <c r="D9" s="19" t="str">
         <f aca="false">IF($A9&lt;&gt;"",($A9*$A9*Calibration!E$17)+($A9*Calibration!E$18)+Calibration!E$19,"")</f>
         <v/>
       </c>
@@ -2565,17 +2941,109 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.75"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">-161.052143*A2*A2+1041.246165*A2+63.805191</f>
+        <v>1234.9999995925</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <f aca="false">-213.724*A2*A2+1561.49*A2-410.8</f>
+        <v>1404.00579</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">-161.052143*A3*A3+1041.246165*A3+63.805191</f>
+        <v>1667.2793263213</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <f aca="false">-213.724*A3*A3+1561.49*A3-410.8</f>
+        <v>2171.7437484</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">-161.052143*A4*A4+1041.246165*A4+63.805191</f>
+        <v>1694.94767308</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">-213.724*A4*A4+1561.49*A4-410.8</f>
+        <v>2436.68744</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <f aca="false">0.00008241*A25*A25+0.005409*A25+1.31808</f>
+        <v>1.57555584</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <f aca="false">0.00008241*A26*A26+0.005409*A26+1.31808</f>
+        <v>2.51322624</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <f aca="false">0.00008241*A27*A27+0.005409*A27+1.31808</f>
+        <v>3.80582976</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2583,5 +3051,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Windsor lunctime running well
</commit_message>
<xml_diff>
--- a/2016CompetitionBot/Documentation/Camera Calibration Worksheet.xlsx
+++ b/2016CompetitionBot/Documentation/Camera Calibration Worksheet.xlsx
@@ -39,6 +39,9 @@
     <t xml:space="preserve">Trial B</t>
   </si>
   <si>
+    <t xml:space="preserve">Waterloo trial</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
@@ -70,9 +73,6 @@
   </si>
   <si>
     <t xml:space="preserve">Right Side</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unsure</t>
   </si>
   <si>
     <t xml:space="preserve">Valid Points</t>
@@ -142,9 +142,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -303,7 +304,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -373,6 +374,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -566,19 +571,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.64</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.53</c:v>
+                  <c:v>2.54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8</c:v>
+                  <c:v>3.68</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.43</c:v>
+                  <c:v>3.48</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.45</c:v>
+                  <c:v>1.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -590,135 +595,30 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>97</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>99.5</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>106</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.5</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Calibration!$G$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Trial B</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="99ccff"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="99ccff"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="9360">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Calibration!$H$8:$H$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.53</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.51</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Calibration!$I$8:$I$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>103.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>112.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="43617238"/>
-        <c:axId val="14506823"/>
+        <c:axId val="77646711"/>
+        <c:axId val="37102844"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43617238"/>
+        <c:axId val="77646711"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -792,12 +692,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14506823"/>
+        <c:crossAx val="37102844"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="14506823"/>
+        <c:axId val="37102844"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -881,7 +781,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43617238"/>
+        <c:crossAx val="77646711"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1037,19 +937,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>33.5</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>144</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1061,19 +961,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.64</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.53</c:v>
+                  <c:v>2.54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8</c:v>
+                  <c:v>3.68</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.43</c:v>
+                  <c:v>3.48</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.45</c:v>
+                  <c:v>1.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1143,19 +1043,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>94.5</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>136.5</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1167,30 +1067,30 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.7</c:v>
+                  <c:v>1.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.51</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>1.43</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>1.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="40630086"/>
-        <c:axId val="13225937"/>
+        <c:axId val="29762858"/>
+        <c:axId val="15375846"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40630086"/>
+        <c:axId val="29762858"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1264,12 +1164,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13225937"/>
+        <c:crossAx val="15375846"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="13225937"/>
+        <c:axId val="15375846"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1353,7 +1253,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40630086"/>
+        <c:crossAx val="29762858"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1509,19 +1409,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.64</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.53</c:v>
+                  <c:v>2.54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8</c:v>
+                  <c:v>3.68</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.43</c:v>
+                  <c:v>3.48</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.45</c:v>
+                  <c:v>1.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1533,10 +1433,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>1110</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>1340</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v/>
@@ -1545,7 +1445,7 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1615,19 +1515,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.7</c:v>
+                  <c:v>1.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.51</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.43</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>1.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1658,11 +1558,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="44544726"/>
-        <c:axId val="18008626"/>
+        <c:axId val="63313953"/>
+        <c:axId val="71461792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44544726"/>
+        <c:axId val="63313953"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1736,12 +1636,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18008626"/>
+        <c:crossAx val="71461792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="18008626"/>
+        <c:axId val="71461792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1825,7 +1725,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44544726"/>
+        <c:crossAx val="63313953"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2035,11 +1935,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="47527606"/>
-        <c:axId val="65008430"/>
+        <c:axId val="6608323"/>
+        <c:axId val="72577775"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47527606"/>
+        <c:axId val="6608323"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2074,12 +1974,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65008430"/>
+        <c:crossAx val="72577775"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65008430"/>
+        <c:axId val="72577775"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2123,7 +2023,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47527606"/>
+        <c:crossAx val="6608323"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2167,13 +2067,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>14400</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>532440</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2181,8 +2081,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14400" y="3943080"/>
-        <a:ext cx="4853520" cy="2742120"/>
+        <a:off x="14400" y="3927960"/>
+        <a:ext cx="5265000" cy="2741760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2195,15 +2095,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>19080</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:colOff>3600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>503640</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:colOff>487440</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>134640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2211,8 +2111,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4979520" y="3943080"/>
-        <a:ext cx="4904280" cy="2742120"/>
+        <a:off x="5383080" y="3785760"/>
+        <a:ext cx="4949280" cy="2741760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2241,8 +2141,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="6791040"/>
-        <a:ext cx="4853520" cy="2742480"/>
+        <a:off x="0" y="6775920"/>
+        <a:ext cx="5265000" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2266,9 +2166,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>240120</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>97920</xdr:rowOff>
+      <xdr:rowOff>97560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2276,8 +2176,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1910880" y="36000"/>
-        <a:ext cx="5827680" cy="3239280"/>
+        <a:off x="1933560" y="36000"/>
+        <a:ext cx="5896080" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2298,23 +2198,19 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.015306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.4132653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6071428571429"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.10204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="11.015306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.39795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="11.1224489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.6071428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,37 +2237,40 @@
         <v>4</v>
       </c>
       <c r="M5" s="2"/>
+      <c r="O5" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="K6" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
@@ -2382,29 +2281,29 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="4"/>
@@ -2412,10 +2311,10 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2423,35 +2322,43 @@
         <v>1</v>
       </c>
       <c r="B8" s="6" t="n">
-        <v>1.64</v>
+        <v>1.6</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>33.5</v>
-      </c>
-      <c r="E8" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>1110</v>
+      </c>
       <c r="G8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H8" s="6" t="n">
-        <v>1.7</v>
+        <v>1.64</v>
       </c>
       <c r="I8" s="6" t="n">
-        <v>103.5</v>
+        <v>97</v>
       </c>
       <c r="J8" s="6" t="n">
-        <v>35</v>
+        <v>33.5</v>
       </c>
       <c r="K8" s="6"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
+      <c r="N8" s="6" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="O8" s="6" t="n">
+        <v>103.5</v>
+      </c>
+      <c r="P8" s="6" t="n">
+        <v>35</v>
+      </c>
       <c r="Q8" s="6"/>
       <c r="R8" s="0" t="n">
-        <v>5140</v>
+        <v>5365</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2459,15 +2366,17 @@
         <v>2</v>
       </c>
       <c r="B9" s="6" t="n">
-        <v>2.53</v>
+        <v>2.54</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>99.5</v>
+        <v>109</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>92</v>
-      </c>
-      <c r="E9" s="6"/>
+        <v>91</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>1340</v>
+      </c>
       <c r="G9" s="5" t="n">
         <v>2</v>
       </c>
@@ -2475,22 +2384,28 @@
         <v>2.53</v>
       </c>
       <c r="I9" s="6" t="n">
-        <v>112.5</v>
+        <v>99.5</v>
       </c>
       <c r="J9" s="6" t="n">
-        <v>94.5</v>
+        <v>92</v>
       </c>
       <c r="K9" s="6"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="N9" s="6" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="O9" s="6" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="P9" s="6" t="n">
+        <v>94.5</v>
+      </c>
       <c r="Q9" s="6"/>
       <c r="R9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="S9" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="S9" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2498,35 +2413,41 @@
         <v>3</v>
       </c>
       <c r="B10" s="6" t="n">
-        <v>3.8</v>
+        <v>3.68</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E10" s="6"/>
       <c r="G10" s="5" t="n">
         <v>3</v>
       </c>
       <c r="H10" s="6" t="n">
-        <v>3.51</v>
+        <v>3.8</v>
       </c>
       <c r="I10" s="6" t="n">
-        <v>107.5</v>
+        <v>106</v>
       </c>
       <c r="J10" s="6" t="n">
-        <v>136.5</v>
+        <v>144</v>
       </c>
       <c r="K10" s="6"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
+      <c r="N10" s="6" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="O10" s="6" t="n">
+        <v>107.5</v>
+      </c>
+      <c r="P10" s="6" t="n">
+        <v>136.5</v>
+      </c>
       <c r="Q10" s="6"/>
       <c r="R10" s="0" t="n">
-        <v>5432</v>
+        <v>-5429</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2534,21 +2455,23 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="n">
-        <v>1.43</v>
-      </c>
-      <c r="C11" s="6" t="n">
-        <v>85</v>
-      </c>
-      <c r="D11" s="6" t="n">
-        <v>12</v>
-      </c>
+        <v>3.48</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="G11" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="H11" s="6" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="I11" s="6" t="n">
+        <v>85</v>
+      </c>
+      <c r="J11" s="6" t="n">
+        <v>12</v>
+      </c>
       <c r="K11" s="6"/>
       <c r="M11" s="5"/>
       <c r="N11" s="6"/>
@@ -2561,24 +2484,25 @@
         <v>5</v>
       </c>
       <c r="B12" s="6" t="n">
-        <v>1.45</v>
-      </c>
-      <c r="C12" s="6" t="n">
-        <v>79.5</v>
-      </c>
-      <c r="D12" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="0" t="s">
-        <v>16</v>
+        <v>1.35</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6" t="n">
+        <v>1000</v>
       </c>
       <c r="G12" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="H12" s="6" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="I12" s="6" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="J12" s="6" t="n">
+        <v>29</v>
+      </c>
       <c r="K12" s="6"/>
       <c r="M12" s="5"/>
       <c r="N12" s="6"/>
@@ -2586,22 +2510,22 @@
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="9" t="n">
         <f aca="false">COUNT(C8:C12)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13" s="9" t="n">
         <f aca="false">COUNT(D8:D12)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E13" s="9" t="n">
         <f aca="false">COUNT(E8:E12)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>18</v>
@@ -2609,11 +2533,11 @@
       <c r="H13" s="8"/>
       <c r="I13" s="9" t="n">
         <f aca="false">COUNT(I8:I12)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J13" s="9" t="n">
         <f aca="false">COUNT(J8:J12)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K13" s="9" t="n">
         <f aca="false">COUNT(K8:K12)</f>
@@ -2657,13 +2581,13 @@
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="12" t="s">
@@ -2671,13 +2595,13 @@
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N16" s="16" t="s">
         <v>23</v>
@@ -2691,9 +2615,9 @@
       <c r="C17" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="D17" s="17" t="n">
+      <c r="D17" s="18" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(B8,0,0,D13),OFFSET(D8,0,0,D13)^{1,2}),1)</f>
-        <v>8.24107322300553E-005</v>
+        <v>8.06989462451648E-005</v>
       </c>
       <c r="E17" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(E8,0,0,E13),OFFSET(B8,0,0,E13)^{1,2}),1)</f>
@@ -2709,7 +2633,7 @@
       </c>
       <c r="J17" s="17" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(H8,0,0,J13),OFFSET(J8,0,0,J13)^{1,2}),1)</f>
-        <v>9.24507734128133E-005</v>
+        <v>8.24107322300553E-005</v>
       </c>
       <c r="K17" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(K8,0,0,K13),OFFSET(H8,0,0,K13)^{1,2}),1)</f>
@@ -2726,11 +2650,11 @@
       <c r="B18" s="11"/>
       <c r="C18" s="17" t="n">
         <f aca="true">SLOPE(OFFSET(C8,0,0,C13),OFFSET(B8,0,0,C13))</f>
-        <v>8.96356510378865</v>
-      </c>
-      <c r="D18" s="17" t="n">
+        <v>7.60722625046086</v>
+      </c>
+      <c r="D18" s="18" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(B8,0,0,D13),OFFSET(D8,0,0,D13)^{1,2}),1,2)</f>
-        <v>0.00540917043605021</v>
+        <v>0.00462384953981592</v>
       </c>
       <c r="E18" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(E8,0,0,E13),OFFSET(B8,0,0,E13)^{1,2}),1,2)</f>
@@ -2742,11 +2666,11 @@
       <c r="H18" s="11"/>
       <c r="I18" s="17" t="n">
         <f aca="true">SLOPE(OFFSET(I8,0,0,I13),OFFSET(H8,0,0,I13))</f>
-        <v>1.99171640881959</v>
+        <v>8.96356510378865</v>
       </c>
       <c r="J18" s="17" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(H8,0,0,J13),OFFSET(J8,0,0,J13)^{1,2}),1,2)</f>
-        <v>0.00197720467497345</v>
+        <v>0.00540917043605021</v>
       </c>
       <c r="K18" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(K8,0,0,K13),OFFSET(H8,0,0,K13)^{1,2}),1,2)</f>
@@ -2760,11 +2684,11 @@
       <c r="B19" s="11"/>
       <c r="C19" s="17" t="n">
         <f aca="true">INTERCEPT(OFFSET(C8,0,0,C13),OFFSET(B8,0,0,C13))</f>
-        <v>73.9490637247786</v>
-      </c>
-      <c r="D19" s="17" t="n">
+        <v>87.8371635737987</v>
+      </c>
+      <c r="D19" s="18" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(B8,0,0,D13),OFFSET(D8,0,0,D13)^{1,2}),1,3)</f>
-        <v>1.3180798365994</v>
+        <v>1.45096171802054</v>
       </c>
       <c r="E19" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(E8,0,0,E13),OFFSET(B8,0,0,E13)^{1,2}),1,3)</f>
@@ -2776,11 +2700,11 @@
       <c r="H19" s="11"/>
       <c r="I19" s="17" t="n">
         <f aca="true">INTERCEPT(OFFSET(I8,0,0,I13),OFFSET(H8,0,0,I13))</f>
-        <v>102.694704998579</v>
+        <v>73.9490637247786</v>
       </c>
       <c r="J19" s="17" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(H8,0,0,J13),OFFSET(J8,0,0,J13)^{1,2}),1,3)</f>
-        <v>1.51754563894523</v>
+        <v>1.3180798365994</v>
       </c>
       <c r="K19" s="17" t="e">
         <f aca="true">INDEX(LINEST(OFFSET(K8,0,0,K13),OFFSET(H8,0,0,K13)^{1,2}),1,3)</f>
@@ -2816,9 +2740,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2833,19 +2755,19 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="19" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2853,100 +2775,100 @@
       <c r="A5" s="6" t="n">
         <v>1.5</v>
       </c>
-      <c r="B5" s="19" t="n">
+      <c r="B5" s="20" t="n">
         <f aca="false">IF($A5&lt;&gt;"",($A5*$A5*Calibration!C$17)+($A5*Calibration!C$18)+Calibration!C$19,"")</f>
-        <v>87.3944113804616</v>
-      </c>
-      <c r="C5" s="19" t="n">
+        <v>99.24800294949</v>
+      </c>
+      <c r="C5" s="20" t="n">
         <f aca="false">IF($A5&lt;&gt;"",($A5*$A5*$H$5)+($A5*$H$6)+$H$7,"")</f>
-        <v>24.4722094362834</v>
-      </c>
-      <c r="D5" s="19" t="e">
+        <v>14.2980589772303</v>
+      </c>
+      <c r="D5" s="20" t="e">
         <f aca="false">IF($A5&lt;&gt;"",($A5*$A5*Calibration!E$17)+($A5*Calibration!E$18)+Calibration!E$19,"")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="19" t="n">
+      <c r="H5" s="20" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(Calibration!D8,0,0,Calibration!D13),OFFSET(Calibration!B8,0,0,Calibration!D13)^{1,2}),1)</f>
-        <v>-10.5503267320325</v>
+        <v>-14.1144083613289</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="n">
         <v>2.5</v>
       </c>
-      <c r="B6" s="19" t="n">
+      <c r="B6" s="20" t="n">
         <f aca="false">IF($A6&lt;&gt;"",($A6*$A6*Calibration!C$17)+($A6*Calibration!C$18)+Calibration!C$19,"")</f>
-        <v>96.3579764842503</v>
-      </c>
-      <c r="C6" s="19" t="n">
+        <v>106.855229199951</v>
+      </c>
+      <c r="C6" s="20" t="n">
         <f aca="false">IF($A6&lt;&gt;"",($A6*$A6*$H$5)+($A6*$H$6)+$H$7,"")</f>
-        <v>90.1690115647921</v>
-      </c>
-      <c r="D6" s="19" t="e">
+        <v>88.6145016797313</v>
+      </c>
+      <c r="D6" s="20" t="e">
         <f aca="false">IF($A6&lt;&gt;"",($A6*$A6*Calibration!E$17)+($A6*Calibration!E$18)+Calibration!E$19,"")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="19" t="n">
+      <c r="H6" s="20" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(Calibration!D8,0,0,Calibration!D13),OFFSET(Calibration!B8,0,0,Calibration!D13)^{1,2}),1,2)</f>
-        <v>107.898109056639</v>
+        <v>130.774076147816</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="n">
         <v>3.5</v>
       </c>
-      <c r="B7" s="19" t="n">
+      <c r="B7" s="20" t="n">
         <f aca="false">IF($A7&lt;&gt;"",($A7*$A7*Calibration!C$17)+($A7*Calibration!C$18)+Calibration!C$19,"")</f>
-        <v>105.321541588039</v>
-      </c>
-      <c r="C7" s="19" t="n">
+        <v>114.462455450412</v>
+      </c>
+      <c r="C7" s="20" t="n">
         <f aca="false">IF($A7&lt;&gt;"",($A7*$A7*$H$5)+($A7*$H$6)+$H$7,"")</f>
-        <v>134.765160229236</v>
-      </c>
-      <c r="D7" s="19" t="e">
+        <v>134.702127659575</v>
+      </c>
+      <c r="D7" s="20" t="e">
         <f aca="false">IF($A7&lt;&gt;"",($A7*$A7*Calibration!E$17)+($A7*Calibration!E$18)+Calibration!E$19,"")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="19" t="n">
+      <c r="H7" s="20" t="n">
         <f aca="true">INDEX(LINEST(OFFSET(Calibration!D8,0,0,Calibration!D13),OFFSET(Calibration!B8,0,0,Calibration!D13)^{1,2}),1,3)</f>
-        <v>-113.636719001601</v>
+        <v>-150.105636431504</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6"/>
-      <c r="B8" s="19" t="str">
+      <c r="B8" s="20" t="str">
         <f aca="false">IF($A8&lt;&gt;"",($A8*$A8*Calibration!C$17)+($A8*Calibration!C$18)+Calibration!C$19,"")</f>
         <v/>
       </c>
-      <c r="C8" s="19" t="str">
+      <c r="C8" s="20" t="str">
         <f aca="false">IF($A8&lt;&gt;"",($A8*$A8*$H$5)+($A8*$H$6)+$H$7,"")</f>
         <v/>
       </c>
-      <c r="D8" s="19" t="str">
+      <c r="D8" s="20" t="str">
         <f aca="false">IF($A8&lt;&gt;"",($A8*$A8*Calibration!E$17)+($A8*Calibration!E$18)+Calibration!E$19,"")</f>
         <v/>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6"/>
-      <c r="B9" s="19" t="str">
+      <c r="B9" s="20" t="str">
         <f aca="false">IF($A9&lt;&gt;"",($A9*$A9*Calibration!C$17)+($A9*Calibration!C$18)+Calibration!C$19,"")</f>
         <v/>
       </c>
-      <c r="C9" s="19" t="str">
+      <c r="C9" s="20" t="str">
         <f aca="false">IF($A9&lt;&gt;"",($A9*$A9*$H$5)+($A9*$H$6)+$H$7,"")</f>
         <v/>
       </c>
-      <c r="D9" s="19" t="str">
+      <c r="D9" s="20" t="str">
         <f aca="false">IF($A9&lt;&gt;"",($A9*$A9*Calibration!E$17)+($A9*Calibration!E$18)+Calibration!E$19,"")</f>
         <v/>
       </c>
@@ -2974,9 +2896,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.85714285714286"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>